<commit_message>
Incluindo looping para puxar dados do excel
</commit_message>
<xml_diff>
--- a/requisicoes.xlsx
+++ b/requisicoes.xlsx
@@ -5,28 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsantos\PycharmProjects\automacaoConferenciaVendas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estudos\Python\Aula01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4AE6C5-60F6-43D1-8ECE-9B2E5B54B644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A550E7-1101-4B36-BB55-288CAC2D8128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -36,9 +25,6 @@
     <t>Comprador</t>
   </si>
   <si>
-    <t>CNPJ_Fornecedor</t>
-  </si>
-  <si>
     <t>Quantidade</t>
   </si>
   <si>
@@ -111,7 +97,10 @@
     <t>ID_requisicao</t>
   </si>
   <si>
-    <t>ID_Item</t>
+    <t>CNPJ_fornecedor</t>
+  </si>
+  <si>
+    <t>ID_item</t>
   </si>
 </sst>
 </file>
@@ -174,8 +163,8 @@
     <tableColumn id="1" xr3:uid="{5738A091-E8A3-4BD6-8801-82FC1455435F}" name="BU"/>
     <tableColumn id="2" xr3:uid="{64BE56C1-643A-4192-AAE5-5319D3F56A0F}" name="Titulo"/>
     <tableColumn id="3" xr3:uid="{876BB7A9-A019-4D3B-AB95-A266FFA48351}" name="Comprador"/>
-    <tableColumn id="4" xr3:uid="{D56D0F31-4918-4E45-8E8B-1A54146346DC}" name="CNPJ_Fornecedor"/>
-    <tableColumn id="5" xr3:uid="{5C0EF0EA-E368-40F7-84FF-EADDEDD469F2}" name="ID_Item"/>
+    <tableColumn id="4" xr3:uid="{D56D0F31-4918-4E45-8E8B-1A54146346DC}" name="CNPJ_fornecedor"/>
+    <tableColumn id="5" xr3:uid="{5C0EF0EA-E368-40F7-84FF-EADDEDD469F2}" name="ID_item"/>
     <tableColumn id="6" xr3:uid="{1951DA23-BF06-4665-A9C5-5B84F45BB262}" name="Quantidade"/>
     <tableColumn id="7" xr3:uid="{87F5FDC3-294C-436B-847A-03BD52099ED6}" name="Budge_unidade"/>
     <tableColumn id="8" xr3:uid="{E202EAC2-BE49-47E7-88E7-8A2A1A177621}" name="Valor"/>
@@ -473,7 +462,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,31 +479,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
         <v>26</v>
       </c>
       <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -522,13 +511,13 @@
         <v>21234</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
       <c r="E2">
         <v>1301010324</v>
@@ -545,13 +534,13 @@
         <v>21218</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>2802180406</v>
@@ -571,13 +560,13 @@
         <v>21201</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>2802180406</v>
@@ -597,13 +586,13 @@
         <v>21202</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>2802180406</v>
@@ -623,13 +612,13 @@
         <v>21204</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>2802180406</v>
@@ -649,13 +638,13 @@
         <v>21205</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>2802180406</v>
@@ -675,13 +664,13 @@
         <v>21206</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <v>2802180406</v>
@@ -701,13 +690,13 @@
         <v>21208</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <v>2802180406</v>
@@ -727,13 +716,13 @@
         <v>21210</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <v>2802180406</v>
@@ -753,13 +742,13 @@
         <v>21211</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11">
         <v>2802180406</v>
@@ -779,13 +768,13 @@
         <v>21212</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12">
         <v>2802180406</v>
@@ -805,13 +794,13 @@
         <v>21217</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <v>2802180406</v>
@@ -831,13 +820,13 @@
         <v>21220</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14">
         <v>2802180406</v>
@@ -857,13 +846,13 @@
         <v>21222</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>2802180406</v>
@@ -880,7 +869,7 @@
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>